<commit_message>
added working time in Timetable Jonny
</commit_message>
<xml_diff>
--- a/Timetables/Timetable Jonny.xlsx
+++ b/Timetables/Timetable Jonny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgtha\OneDrive\BBE\Biodex\Timetables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{3C732006-4364-428A-9B76-C09814DEC91C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5CB88F7A-635F-4231-83C1-9DBF2C9ABFC4}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{3C732006-4364-428A-9B76-C09814DEC91C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5D72C918-CAE0-4CF0-A755-F85AB28B29BD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{A730D8CD-244E-400F-8D0D-5BD51D145E37}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -42,22 +42,37 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>31.4.</t>
-  </si>
-  <si>
     <t>18:00-20:15</t>
   </si>
   <si>
     <t>Discussion with purpose on setting up Project goals, Customer requiremnets, sharing platform, workpakages, tasks till next meeting</t>
   </si>
   <si>
-    <t>1.4.</t>
-  </si>
-  <si>
     <t>Writing the minute of group meeting 1, Sending email to Nemec, setting up GitHub</t>
   </si>
   <si>
     <t>11:00-15:00</t>
+  </si>
+  <si>
+    <t>12:00-15:00</t>
+  </si>
+  <si>
+    <t>Learning Git Hub</t>
+  </si>
+  <si>
+    <t>31.04.2020</t>
+  </si>
+  <si>
+    <t>11:00-16:00</t>
+  </si>
+  <si>
+    <t>17:00-19:00</t>
+  </si>
+  <si>
+    <t>Setting up Group Paper, adding User Requirements, Project Goals, Workpackages, Naming conventions</t>
+  </si>
+  <si>
+    <t>Finishing first version of Group Paper, Setting up first Version of Wiki</t>
   </si>
 </sst>
 </file>
@@ -93,8 +108,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -409,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F75A4D-8E25-4647-8BC3-40899CBB101B}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -430,24 +448,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>43925</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>43926</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added working time to Timetable Jonny
</commit_message>
<xml_diff>
--- a/Timetables/Timetable Jonny.xlsx
+++ b/Timetables/Timetable Jonny.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgtha\OneDrive\BBE\Biodex\Timetables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{3C732006-4364-428A-9B76-C09814DEC91C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5D72C918-CAE0-4CF0-A755-F85AB28B29BD}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{3C732006-4364-428A-9B76-C09814DEC91C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D48922D4-9CC4-48B1-BA00-1FCCB6449D54}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{A730D8CD-244E-400F-8D0D-5BD51D145E37}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Finishing first version of Group Paper, Setting up first Version of Wiki</t>
+  </si>
+  <si>
+    <t>18:00-20:30</t>
+  </si>
+  <si>
+    <t>Discussion about progrees last week, writing meeting minute</t>
   </si>
 </sst>
 </file>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F75A4D-8E25-4647-8BC3-40899CBB101B}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -501,6 +507,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>